<commit_message>
Update 221005_VPS 1팀 마일스톤_V100.xlsx
</commit_message>
<xml_diff>
--- a/일정관리/221005_VPS 1팀 마일스톤_V100.xlsx
+++ b/일정관리/221005_VPS 1팀 마일스톤_V100.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>9월</t>
   </si>
@@ -622,7 +622,190 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">10.07 컨셉 기획서 초안 </t>
+    <t xml:space="preserve">10.06 2차 기업 미팅
+10.07 컨셉 기획서 초안 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>기획</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>컨셉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">기획서
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>컨셉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">제안서
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>마일스톤</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, WBS
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>개발</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+구글</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> AR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>기술</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> R&amp;D</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -852,8 +1035,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -895,19 +1081,16 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1836,7 +2019,7 @@
   <dimension ref="B2:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:D6"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1847,29 +2030,29 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B2" s="11"/>
-      <c r="C2" s="19" t="s">
+      <c r="B2" s="12"/>
+      <c r="C2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="12" t="s">
+      <c r="D2" s="21"/>
+      <c r="E2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12" t="s">
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
       <c r="M2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B3" s="11"/>
+      <c r="B3" s="12"/>
       <c r="C3" s="4" t="s">
         <v>13</v>
       </c>
@@ -1905,66 +2088,66 @@
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="15"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="16"/>
     </row>
     <row r="5" spans="2:13" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="10"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="18"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="19"/>
     </row>
     <row r="6" spans="2:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="25" t="s">
+      <c r="D6" s="23"/>
+      <c r="E6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="22"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="8" t="s">
+      <c r="G6" s="25"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="22"/>
-      <c r="K6" s="9"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="10"/>
       <c r="L6" s="6" t="s">
         <v>22</v>
       </c>
       <c r="M6" s="5"/>
     </row>
     <row r="7" spans="2:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="10"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="25" t="s">
+      <c r="B7" s="11"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F7" s="5"/>
@@ -1986,7 +2169,7 @@
       <c r="D8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="8" t="s">
         <v>26</v>
       </c>
       <c r="F8" s="5"/>
@@ -2006,15 +2189,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:13" ht="281.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="5"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>

</xml_diff>